<commit_message>
1. Completed post requests positive tests 2. Minor updates with get requests
Signed-off-by: Avik D <audi4avik@gmail.com>
</commit_message>
<xml_diff>
--- a/Rest API DemoQA/Input Data/TestData.xlsx
+++ b/Rest API DemoQA/Input Data/TestData.xlsx
@@ -9,18 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Positive" sheetId="1" r:id="rId1"/>
-    <sheet name="Negative" sheetId="2" r:id="rId2"/>
+    <sheet name="Get-Positive" sheetId="1" r:id="rId1"/>
+    <sheet name="Get-Negative" sheetId="2" r:id="rId2"/>
+    <sheet name="Post-Positive" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="66">
   <si>
     <t>${TC_No}</t>
   </si>
@@ -140,6 +141,84 @@
   </si>
   <si>
     <t>Chernai</t>
+  </si>
+  <si>
+    <t>http://restapi.demoqa.com/customer</t>
+  </si>
+  <si>
+    <t>/register</t>
+  </si>
+  <si>
+    <t>${firstName}</t>
+  </si>
+  <si>
+    <t>${lastName}</t>
+  </si>
+  <si>
+    <t>${userName}</t>
+  </si>
+  <si>
+    <t>${password}</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Doe</t>
+  </si>
+  <si>
+    <t>jdoe1234</t>
+  </si>
+  <si>
+    <t>JDoe1558</t>
+  </si>
+  <si>
+    <t>${relativeUrl}</t>
+  </si>
+  <si>
+    <t>${email}</t>
+  </si>
+  <si>
+    <t>jdoe@gmail.com</t>
+  </si>
+  <si>
+    <t>OPERATION_SUCCESS</t>
+  </si>
+  <si>
+    <t>Operation completed successfully</t>
+  </si>
+  <si>
+    <t>${successCode}</t>
+  </si>
+  <si>
+    <t>${respMessage}</t>
+  </si>
+  <si>
+    <t>User already exists</t>
+  </si>
+  <si>
+    <t>FAULT_USER_ALREADY_EXISTS</t>
+  </si>
+  <si>
+    <t>Validate registration scenario for existing customer</t>
+  </si>
+  <si>
+    <t>Validate successful registration for new customer</t>
+  </si>
+  <si>
+    <t>new user</t>
+  </si>
+  <si>
+    <t>random email</t>
+  </si>
+  <si>
+    <t>Jane</t>
+  </si>
+  <si>
+    <t>Johnny</t>
+  </si>
+  <si>
+    <t>Depp</t>
   </si>
 </sst>
 </file>
@@ -510,7 +589,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -698,8 +777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -850,4 +929,225 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="45.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="10.81640625" customWidth="1"/>
+    <col min="9" max="9" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="29.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I2">
+        <v>201</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K2" t="s">
+        <v>53</v>
+      </c>
+      <c r="L2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H3" t="s">
+        <v>49</v>
+      </c>
+      <c r="I3">
+        <v>201</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K3" t="s">
+        <v>53</v>
+      </c>
+      <c r="L3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G4" t="s">
+        <v>61</v>
+      </c>
+      <c r="H4" t="s">
+        <v>49</v>
+      </c>
+      <c r="I4">
+        <v>201</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K4" t="s">
+        <v>53</v>
+      </c>
+      <c r="L4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G5" t="s">
+        <v>48</v>
+      </c>
+      <c r="H5" t="s">
+        <v>49</v>
+      </c>
+      <c r="I5">
+        <v>200</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K5" t="s">
+        <v>57</v>
+      </c>
+      <c r="L5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C5" r:id="rId1"/>
+    <hyperlink ref="J5" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+</worksheet>
 </file>
</xml_diff>